<commit_message>
converted to Maven updates
</commit_message>
<xml_diff>
--- a/ADCVD_REGRESSION/input_data/datapool/Regession_TC.xlsx
+++ b/ADCVD_REGRESSION/input_data/datapool/Regession_TC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E829F1-A833-4319-A334-BA736A7C71D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E10F10-9A6C-4DAB-98D8-9A69130523A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2304" windowWidth="19008" windowHeight="7920" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="dropdowns" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Regression!$A$1:$Z$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Regression!$A$1:$AB$14</definedName>
     <definedName name="CaseType">dropdowns!$B$1:$B$2</definedName>
     <definedName name="CaseType2">dropdowns!$E$1:$E$3</definedName>
     <definedName name="FiledSelf">dropdowns!$C$1:$C$2</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="118">
   <si>
     <t>TC_TAG_001</t>
   </si>
@@ -380,6 +380,18 @@
   </si>
   <si>
     <t>Preliminary_Determination</t>
+  </si>
+  <si>
+    <t>Decision_On_How_To_Proceed</t>
+  </si>
+  <si>
+    <t>Formal</t>
+  </si>
+  <si>
+    <t>Type_Of_Scope_Ruling</t>
+  </si>
+  <si>
+    <t>K (1)</t>
   </si>
 </sst>
 </file>
@@ -730,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB8:AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,10 +773,11 @@
     <col min="23" max="23" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="28.5546875" customWidth="1"/>
+    <col min="28" max="28" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -841,10 +854,16 @@
         <v>60</v>
       </c>
       <c r="Z1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -896,11 +915,13 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="1" t="b">
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -940,11 +961,13 @@
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="1" t="b">
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1000,11 +1023,13 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="1" t="b">
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1060,11 +1085,13 @@
       <c r="Y5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Z5" s="1" t="b">
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1118,11 +1145,13 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="1" t="b">
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1176,11 +1205,13 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="1" t="b">
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1238,11 +1269,13 @@
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1" t="b">
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1302,11 +1335,13 @@
       <c r="Y9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Z9" s="1" t="b">
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1364,11 +1399,13 @@
       </c>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="1" t="b">
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1430,11 +1467,13 @@
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="1" t="b">
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1498,11 +1537,13 @@
       </c>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1564,11 +1605,17 @@
       </c>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB13" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1626,12 +1673,14 @@
       </c>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="1" t="b">
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z14" xr:uid="{F0E771B3-A481-4DD0-B3ED-7DCB6749EF64}"/>
+  <autoFilter ref="A1:AB14" xr:uid="{F0E771B3-A481-4DD0-B3ED-7DCB6749EF64}"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 M4:M14" xr:uid="{6A157A86-3C6C-4079-A49E-09147802FCCC}">
       <formula1>Yes_No</formula1>
@@ -1642,7 +1691,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2 H4:H14" xr:uid="{46AD7191-82B7-413F-8595-7A1128BA42E7}">
       <formula1>CaseType2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z14" xr:uid="{DBE1DED1-53EF-43BE-8D71-88C6B8A3A55F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB14" xr:uid="{DBE1DED1-53EF-43BE-8D71-88C6B8A3A55F}">
       <formula1>tFalse</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E14" xr:uid="{226BB8D3-1623-478B-A6C3-89622019E118}">

</xml_diff>

<commit_message>
adding api and access
</commit_message>
<xml_diff>
--- a/ADCVD_REGRESSION/input_data/datapool/Regession_TC.xlsx
+++ b/ADCVD_REGRESSION/input_data/datapool/Regession_TC.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB48994-1191-4790-83DE-C6F3C5E45384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BB09C3-2B94-4098-822D-B4636B461F2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="2310" windowWidth="19005" windowHeight="7920" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2316" windowWidth="19008" windowHeight="7920" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
@@ -862,38 +862,38 @@
   <dimension ref="A1:AC17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD18" sqref="AD18"/>
+      <selection activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="16" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="45.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="34.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="45.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="34.44140625" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="25" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" hidden="1" customWidth="1"/>
-    <col min="19" max="22" width="18.5703125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="27.140625" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="31.85546875" hidden="1" customWidth="1"/>
-    <col min="25" max="27" width="28.5703125" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="6.28515625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" hidden="1" customWidth="1"/>
+    <col min="19" max="22" width="18.5546875" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="27.109375" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="31.88671875" hidden="1" customWidth="1"/>
+    <col min="25" max="27" width="28.5546875" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="19.44140625" customWidth="1"/>
     <col min="29" max="29" width="63" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -982,7 +982,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1037,13 +1037,13 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC2" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1086,13 +1086,13 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="6"/>
       <c r="AB3" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC3" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1151,13 +1151,13 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1216,13 +1216,13 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="6"/>
       <c r="AB5" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1279,13 +1279,13 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1341,14 +1341,14 @@
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="9"/>
-      <c r="AB7" s="9" t="b">
+      <c r="AB7" s="16" t="b">
         <v>0</v>
       </c>
       <c r="AC7" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1408,14 +1408,14 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="1" t="b">
+      <c r="AB8" s="6" t="b">
         <v>1</v>
       </c>
       <c r="AC8" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1477,14 +1477,14 @@
       </c>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-      <c r="AB9" s="1" t="b">
+      <c r="AB9" s="6" t="b">
         <v>1</v>
       </c>
       <c r="AC9" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1544,14 +1544,14 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="1" t="b">
+      <c r="AB10" s="6" t="b">
         <v>1</v>
       </c>
       <c r="AC10" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1615,14 +1615,14 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-      <c r="AB11" s="1" t="b">
+      <c r="AB11" s="6" t="b">
         <v>1</v>
       </c>
       <c r="AC11" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1688,14 +1688,14 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="1" t="b">
+      <c r="AB12" s="6" t="b">
         <v>1</v>
       </c>
       <c r="AC12" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1763,14 +1763,14 @@
       <c r="AA13" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AB13" s="1" t="b">
-        <v>1</v>
+      <c r="AB13" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AC13" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1830,14 +1830,14 @@
       <c r="Y14" s="11"/>
       <c r="Z14" s="11"/>
       <c r="AA14" s="11"/>
-      <c r="AB14" s="12" t="b">
+      <c r="AB14" s="16" t="b">
         <v>0</v>
       </c>
       <c r="AC14" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1881,14 +1881,14 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
       <c r="AA15" s="14"/>
-      <c r="AB15" s="12" t="b">
-        <v>0</v>
+      <c r="AB15" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="AC15" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -1932,14 +1932,14 @@
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
-      <c r="AB16" s="12" t="b">
-        <v>1</v>
+      <c r="AB16" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AC16" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:AB14" xr:uid="{F0E771B3-A481-4DD0-B3ED-7DCB6749EF64}"/>
   <dataValidations count="5">
@@ -1972,12 +1972,12 @@
       <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>32</v>
       </c>
@@ -2054,22 +2054,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F5" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F7" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F8" s="2" t="s">
         <v>40</v>
       </c>

</xml_diff>